<commit_message>
added pytests for inputs urls, filters, extensions, groups
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -13,65 +13,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
-  <si>
-    <t>interface</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>mask</t>
-  </si>
-  <si>
-    <t>vrf</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Loopback0</t>
-  </si>
-  <si>
-    <t>192.168.0.113</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Router-id-loopback</t>
-  </si>
-  <si>
-    <t>Loopback1</t>
-  </si>
-  <si>
-    <t>192.168.0.1</t>
-  </si>
-  <si>
-    <t>Vlan778</t>
-  </si>
-  <si>
-    <t>2002::fd37</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>CPE1</t>
-  </si>
-  <si>
-    <t>Vlan779</t>
-  </si>
-  <si>
-    <t>2002::bbcd</t>
-  </si>
-  <si>
-    <t>CPE2</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -113,6 +54,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,53 +422,80 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>interface</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mask</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vrf</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Loopback0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.0.113</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Router-id-loopback</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s"/>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Loopback1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.0.1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Router-id-loopback</t>
+        </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -477,47 +513,72 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>interface</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mask</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vrf</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vlan778</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2002::fd37</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CPE1</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Vlan779</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2002::bbcd</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CPE2</t>
+        </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved input sources to separate directory; added docs and new attributes for syslog returner;
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ficed csv formater to use quote character to enclode values, that is to properly handle case when have commas on values; added new attribute to csv formatter - quote - to specify quote character to use; updated docs
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated readme; updated setup.py with new version
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added TTP internal docs section; fixed bug in form_result function with _anonymous_ key double pop
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug with file returner not properly handling raw data
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test for add fun for match, group and input, added support for custom function to multiprocesing mode
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support to supply structured data - list or dictionary - asinput data, so that macro can be used within input to pre-process it
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 'vars' keyword in _ttp_ dictionary to reference in run <vars> tag variables instead of _ttp_['reslts_object'].vars
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed major pylint errors
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated input attributes docs to give a bit cleaner description of groups mapping logic
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
blackened the code and fixed some minor issues like unused imports or unusedvariables across various functions
</commit_message>
<xml_diff>
--- a/test/pytest/Output/excel_out_test_excel_formatter.xlsx
+++ b/test/pytest/Output/excel_out_test_excel_formatter.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="loopbacks" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -495,7 +495,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -579,6 +579,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>